<commit_message>
Add Table Reviewer 1
</commit_message>
<xml_diff>
--- a/Data/3. Alkalinity/Alkalinity_setup/Alk_pH_calculations.xlsx
+++ b/Data/3. Alkalinity/Alkalinity_setup/Alk_pH_calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/3. Alkalinity/Alkalinity_setup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremycarlot/Documents/Post-Doc – LOV/Projets/Villefranche/Projets/BenthFun – Jeremy (pending)/BenthFun/Data/3. Alkalinity/Alkalinity_setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E96260-B5BB-C249-87AB-CF1F94B2B46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090F34F0-9CE3-2F42-AECD-450F014B76D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -228,14 +231,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -577,7 +579,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,16 +623,16 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>10.01</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>7</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>35</v>
       </c>
     </row>
@@ -638,32 +640,32 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>-180.7</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>-5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="13">
-        <v>20</v>
+      <c r="F6" s="12">
+        <v>22.3</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>2.3699999999990951E-3</v>
       </c>
       <c r="H7" t="s">
@@ -671,34 +673,34 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <f>(C6-B6)/(B5-C5)</f>
         <v>58.372093023255815</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="10"/>
       <c r="H8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <f>(B8/59.16)*100</f>
         <v>98.668176171832016</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f>(11911.08 - 18.2499*F5 - 0.039336*F5^2)/(F6 + 273.15) + (-366.27059 + 0.53993607*F5 + 0.00016329*F5^2) + (64.52243 - 0.084041*F5)*LN(F6+273.15) - 0.11149858*(F6+273.15)  +  F7</f>
-        <v>8.2540302486944057</v>
-      </c>
-      <c r="H9" s="8" t="s">
+        <v>8.1807884982660113</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>